<commit_message>
Sign Up Module Started
--2020/03/20
</commit_message>
<xml_diff>
--- a/src/test/java/ExcelFiles/sellerOpticsAppKeywords.xlsx
+++ b/src/test/java/ExcelFiles/sellerOpticsAppKeywords.xlsx
@@ -9,10 +9,11 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="330" yWindow="330" windowWidth="18000" windowHeight="9480"/>
+    <workbookView xWindow="330" yWindow="330" windowWidth="18000" windowHeight="9480" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="Sign In Module" sheetId="1" r:id="rId1"/>
+    <sheet name="Sign Up Module" sheetId="2" r:id="rId2"/>
   </sheets>
   <calcPr calcId="152511"/>
   <extLst>
@@ -30,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="10" uniqueCount="10">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="18" uniqueCount="14">
   <si>
     <t>ID</t>
   </si>
@@ -60,6 +61,18 @@
   </si>
   <si>
     <t>//*[@id="doLogin"]/div[2]/div[4]/div/button</t>
+  </si>
+  <si>
+    <t>//a[contains(text(),'Sign Up')]</t>
+  </si>
+  <si>
+    <t>Sign Up Button</t>
+  </si>
+  <si>
+    <t>//button[@class='btn btn-primary smtBtn']</t>
+  </si>
+  <si>
+    <t>Continue to Sign Up Screen</t>
   </si>
 </sst>
 </file>
@@ -432,8 +445,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:D4"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A4" sqref="A4"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="C18" sqref="C18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -491,4 +504,62 @@
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" horizontalDpi="90" verticalDpi="90" r:id="rId1"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:D4"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="D6" sqref="D6"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="25.28515625" bestFit="1" customWidth="1"/>
+    <col min="2" max="3" width="12" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="41.85546875" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:4" s="2" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A1" s="3" t="s">
+        <v>3</v>
+      </c>
+      <c r="B1" s="3" t="s">
+        <v>2</v>
+      </c>
+      <c r="C1" s="3" t="s">
+        <v>0</v>
+      </c>
+      <c r="D1" s="3" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
+        <v>11</v>
+      </c>
+      <c r="B2" s="1"/>
+      <c r="C2" s="1"/>
+      <c r="D2" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
+        <v>13</v>
+      </c>
+      <c r="B3" s="1"/>
+      <c r="C3" s="1"/>
+      <c r="D3" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="B4" s="1"/>
+      <c r="C4" s="1"/>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>